<commit_message>
Finished documenting time disjunctures. Now cleaning up time discrepancies.
</commit_message>
<xml_diff>
--- a/clean_chrr-wphi/output/my_dictionary_v2.xlsx
+++ b/clean_chrr-wphi/output/my_dictionary_v2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="809">
   <si>
     <t>variable</t>
   </si>
@@ -66,7 +66,7 @@
     <t>longitudinal_data_notes</t>
   </si>
   <si>
-    <t>time_trend_visual_inspection</t>
+    <t>time_trend_decision</t>
   </si>
   <si>
     <t>premature_death</t>
@@ -681,7 +681,7 @@
     <t>preventable_hospital_stays</t>
   </si>
   <si>
-    <t xml:space="preserve">Rate of hospital stays for ambulatory-care sensitive conditions per 1,000 Medicare enrollees.</t>
+    <t xml:space="preserve">Rate of hospital stays for ambulatory-care sensitive conditions per 100,000 Medicare enrollees.</t>
   </si>
   <si>
     <t>mmdt</t>
@@ -699,7 +699,7 @@
     <t xml:space="preserve">The denominator is the number of Medicare beneficiaries ages 18 years or older continuously enrolled in Medicare fee-for-service Part A.</t>
   </si>
   <si>
-    <t xml:space="preserve">From 2019-2023, I change the estimate back to per 1,000 to make results comparable.</t>
+    <t xml:space="preserve">From 2019-2023, I change the estimates to per 1,000 to make results more comparable to earlier releases.</t>
   </si>
   <si>
     <t xml:space="preserve">Individuals must have been hospitalized with one of the following conditions: diabetes with short or long-term complications, uncontrolled diabetes without complications, diabetes with lower-extremity amputation, chronic obstructive pulmonary disease, asthma, hypertension, heart failure, dehydration, bacterial pneumonia, or urinary tract infection. Individuals enrolled in Medicare Advantage at any point during the year are excluded. In addition, beneficiaries who died during the year, but otherwise were continuously enrolled up until the date of death, as well as beneficiaries who became eligible for enrollment following the first of the year, but were continuously enrolled from that date to the end of the year, are included in the analysis population.</t>
@@ -1566,6 +1566,9 @@
     <t xml:space="preserve">Data provider does not recommend using this data to track progress due to concerns that many providers are no longer practicing but are not delisted from the directory. Additionally, the data provider discovered an error in their estimates from 2014-2016 where organizations were being counted alongside individual providers. The corrected estimates were provided in 2015 and 2016 but not 2014. Thus, there are no estimates available for 2014. If one truly wishes to make cross-time comparisons, it appears as if one should use 2015-2023.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are no major discernible disjunctures in the data.</t>
+  </si>
+  <si>
     <t>high_school_graduation</t>
   </si>
   <si>
@@ -1596,6 +1599,9 @@
     <t xml:space="preserve">Data provider does not recommend using this data to track progress. Constant changes in the data source combined with different definitions of the variable across states (even for schools within the same state) make comparisons hard. If one wishes to compare across time, the data provider recommends the following time comparisons: 2010; 2011; 2012-2013; 2014-2018; 2019; 2020; 2021-2023. In particular, the data provider notes that in 2019 the priority was to use state-specific sources for states that had a large number of missing counties in the national-level data. Moving forward, the data provider tried to rely less upon state-level sources and only use the national-level data. When making cross-time comparisons, one should strive to ensure the data sources are the same for all observations.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are no major discernible disjunctures in the data. One state had a huge spike from 2011 to 2012 and achieved a 100% high school graduation rate fro 2012 to 2013 which is most likely a data error.</t>
+  </si>
+  <si>
     <t>disconnected_youth</t>
   </si>
   <si>
@@ -1614,6 +1620,9 @@
     <t xml:space="preserve">Data provider recommends the following time comparisons: 2017-2018; 2019-2023.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a very large, uniform, relative decline from 2018 to 2019.</t>
+  </si>
+  <si>
     <t>reading_scores</t>
   </si>
   <si>
@@ -1632,6 +1641,9 @@
     <t xml:space="preserve">Reading Scores is the average grade level performance in the county for 3rd graders on English Language Arts standardized tests. For example, a score of 3.5 indicates that the 3rd graders are performing half a grade level better than expected for 3rd graders. </t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 4 data points available for this variable and three out of the four data points exhibit no variation (they are the same value).</t>
+  </si>
+  <si>
     <t>math_scores</t>
   </si>
   <si>
@@ -1659,6 +1671,9 @@
     <t xml:space="preserve">School segregation is measured using Thell's index which ranges from 0 to 1 with lower values representing a school composition that approximates race and ethnicity distributions in the student populations within the county and higher values representing more segregation. Data is not collected on private schools.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 2 data points available for this variable.</t>
+  </si>
+  <si>
     <t>school_funding_adequacy</t>
   </si>
   <si>
@@ -1719,6 +1734,9 @@
     <t xml:space="preserve">Childcare cost data are based on market-rate surveys reported separately by state, published in different years. Some states only report state or region-level estimates, and thus require county-level imputation. Due to this, states may differ in the extent to which estimates are modeled vs. observed. I think, primarily for this reason, the data provider suggests caution when comparing this data across time as well across states.</t>
   </si>
   <si>
+    <t xml:space="preserve">In what is likely an error on the data provider's part, all values for this variable are missing.</t>
+  </si>
+  <si>
     <t>children_eligible_for_free_lunch</t>
   </si>
   <si>
@@ -1740,6 +1758,9 @@
     <t xml:space="preserve">There is some discrepancy in the documentation concerning the source of the data. This makes it hard to say which years can be compared with which other years.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a large, uniform, relative increase from 2012 to 2013. From 2014 to 2015 and then 2015 to 2016, several states exhibit large variation (values which jump around quite a bit).</t>
+  </si>
+  <si>
     <t>children_eligible_for_free_or_reduced_price_lunch</t>
   </si>
   <si>
@@ -1755,6 +1776,9 @@
     <t xml:space="preserve">Children eligible for free lunch live in a family with income less than 130% of the federal poverty level, while children eligible for reduced price lunch live in a family with income less than 185% of the federal poverty level.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are a few states which exhibit a large amount of variation otherwise there are no obvious disjunctures.</t>
+  </si>
+  <si>
     <t>residential_segregation_-_black/white</t>
   </si>
   <si>
@@ -1767,13 +1791,19 @@
     <t xml:space="preserve">The degree to which two or more groups live separately from one another in a geographic area. The index of dissimiliarity is a measure of evenness with which two groups are distributed across component geographic areas (census tracts in this case) that make up a larger areas (counties in this case).</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a moderate, uniform, relative increase in values from 2021 to 2022.</t>
+  </si>
+  <si>
     <t>residential_segregation_-_non-white/white</t>
   </si>
   <si>
     <t xml:space="preserve">Index of dissimilarity where higher values indicate greater residential segregation between non-White and White county residents.</t>
   </si>
   <si>
-    <t>childcare_cost_burden</t>
+    <t xml:space="preserve">There is a moderate, heterogeneous, relative increase in values from 2021 to 2022.</t>
+  </si>
+  <si>
+    <t>child_care_cost_burden</t>
   </si>
   <si>
     <t xml:space="preserve">Childcare costs for a household with two children as a percent of median household income.</t>
@@ -1791,13 +1821,19 @@
     <t xml:space="preserve">Median household income data calculated from the Small Area Income and Poverty Estimates.</t>
   </si>
   <si>
+    <t xml:space="preserve">I change this variable from childcare_cost_burden to child_care_cost_burden in 2022 to match later releases of the data.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Living Wage Calculator established child care costs for each county based on market rate surveys published by each state, databases of local providers, and by contacting providers in a state directly.</t>
   </si>
   <si>
     <t xml:space="preserve">Childcare cost data are based on market-rate surveys reported separately by state, published in different years. Some states only report state or region-level estimates, and thus require county-level imputation. Due to this, states may differ in the extent to which estimates are modeled vs. observed. Additionally, the estimate of child care costs have been adjusted to reflect inflation. For both of these reasons, the data provider does not recommend comparing these estimates across year (and also warn of the difficulties of making cross-state comparisons as well).</t>
   </si>
   <si>
-    <t>childcare_centers</t>
+    <t xml:space="preserve">There are only 2 data points available for this variable, and there are no obvious, discernible disjunctures.</t>
+  </si>
+  <si>
+    <t>child_care_centers</t>
   </si>
   <si>
     <t xml:space="preserve">Number of childcare centers per 1,000 population under 5 years old. </t>
@@ -1815,12 +1851,18 @@
     <t xml:space="preserve">The denominator is the total resident population under 5 years old in a county.</t>
   </si>
   <si>
+    <t xml:space="preserve">I change this variable from childcare_centers to child_care_centers in 2022 to match later releases of the data.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The dataset only includes center based child day care locations (including those located at schools and religious institutes) and does not include group, home, and family based child day cares. All the data was acquired from respective states departments or their open source websites and only contains data provided by these sources. Child care centers are regulated by state licensing. Definitions of childcare facilities vary by state making comparisons across states difficult. Data were acquired from respective state's departments and therefore may be subject to reporting differences.</t>
   </si>
   <si>
     <t xml:space="preserve">The data provider does not give any warnings when comparing across time, but they do give a strong warning when comparing across states. See the note in variable_definitions.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 2 data points available for this variable. A few states exhibit a relatively large amount of variation, but most states exhibit stable trends. </t>
+  </si>
+  <si>
     <t>homicides</t>
   </si>
   <si>
@@ -1839,6 +1881,9 @@
     <t xml:space="preserve">It is important to note that deaths are counted in the county of residence of the deceased. So, even if a homicide occurred across the state, the death is counted in the home county of the individual who died. Homicides are defined by ICD-10 codes X85-Y09 (assault).</t>
   </si>
   <si>
+    <t xml:space="preserve">Several states exhibit a large amount of variation otherwise there are no obvious disjunctures.</t>
+  </si>
+  <si>
     <t>suicides</t>
   </si>
   <si>
@@ -1863,6 +1908,9 @@
     <t xml:space="preserve">From 2020-2023, I set the stem for this variable to be raw_value.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are no obvious, discernible disjunctures.</t>
+  </si>
+  <si>
     <t>firearm_fatalities</t>
   </si>
   <si>
@@ -1905,6 +1953,9 @@
     <t xml:space="preserve">The data provider does not give any specific instructions probably because this variable is not used in the rankings. However, I would recommend the following year comparisons: 2010-2012; 2013-2023.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a moderate, (relatively) uniform, relative decline in values from 2012 to 2013.</t>
+  </si>
+  <si>
     <t>juvenile_arrests</t>
   </si>
   <si>
@@ -1989,6 +2040,9 @@
     <t xml:space="preserve">Data provider does not recommend comparing across states due to differences in state collection and reporting of traffic. Data provider does not recommend comparing across time to measure progress.</t>
   </si>
   <si>
+    <t xml:space="preserve">Several states exhibit a great deal of variation for this variable. Otherwise, there are no discernible, obvious disjunctures.</t>
+  </si>
+  <si>
     <t>homeownership</t>
   </si>
   <si>
@@ -2043,6 +2097,9 @@
     <t xml:space="preserve">Presumably, the number of citizens 18 and older, bu there is no concreate documentation.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is only 1 data point available for this variable.</t>
+  </si>
+  <si>
     <t>census_participation</t>
   </si>
   <si>
@@ -2166,6 +2223,9 @@
     <t xml:space="preserve">Number of individuals not proficient in English.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a large, uniform, relative decline in values from 2012 to 2013.</t>
+  </si>
+  <si>
     <t>%_female</t>
   </si>
   <si>
@@ -2178,6 +2238,9 @@
     <t xml:space="preserve">From 2011 to 2021, I rename the variable from %_females to %_female for consistency purposes with newer releases of the data.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a moderate, (relatively) uniform, relative decline in values from 2012 to 2013. There is a large, uniform, relative decline in values from 2022 to 2023.</t>
+  </si>
+  <si>
     <t>%_rural</t>
   </si>
   <si>
@@ -2187,12 +2250,18 @@
     <t xml:space="preserve">Number of individuals living in rural areas.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a large, (relatively) uniform, relative decline in values from 2012 to 2013. Additionally, there is a not a lot of variation in this variable.</t>
+  </si>
+  <si>
     <t>could_not_see_doctor_due_to_cost</t>
   </si>
   <si>
     <t xml:space="preserve">This variable is not used in the rankings so documentation is more sparse. Based on how previous variables from this data source were constructed, it would seem as if all years of availability for this variable could be compared, but this is an informed guess.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a large, (relatively) uniform, relative increase in values from 2013 to 2014.</t>
+  </si>
+  <si>
     <t>high_housing_costs</t>
   </si>
   <si>
@@ -2211,6 +2280,9 @@
     <t>access_to_parks</t>
   </si>
   <si>
+    <t xml:space="preserve">There is only 1 data point available for this variable, and it stopped being updated in 2013.</t>
+  </si>
+  <si>
     <t>illiteracy</t>
   </si>
   <si>
@@ -2220,6 +2292,9 @@
     <t xml:space="preserve">National Center for Education Statistics's National Assessment of Adult Literacy</t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 2 data points available for this variable which exibhit no variation, and it stopped being updated in 2012.</t>
+  </si>
+  <si>
     <t>liquor_store_density</t>
   </si>
   <si>
@@ -2241,6 +2316,9 @@
     <t xml:space="preserve">Liquor stores are defined using NAICS code 445310.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 2 data points available for this variable. A few states exhibit a great deal of variation while most states exhibit very little variation. It stopped being updated in 2011.</t>
+  </si>
+  <si>
     <t>diabetes_monitoring</t>
   </si>
   <si>
@@ -2253,12 +2331,18 @@
     <t xml:space="preserve">The number of diabetic Medicare enrolless ages 65-75.</t>
   </si>
   <si>
+    <t xml:space="preserve">A few states exhibit a great deal of variation while most states exhibit very little variation.</t>
+  </si>
+  <si>
     <t>hospice_use</t>
   </si>
   <si>
     <t xml:space="preserve">Percent of chronically ill Medicare enrollees admitted to hospice in last 6 months of life.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is only 1 data point available for this variable, and it stopped being updated in 2010.</t>
+  </si>
+  <si>
     <t>college_degrees</t>
   </si>
   <si>
@@ -2280,6 +2364,9 @@
     <t xml:space="preserve">The number of adults reporting they do not get social/emotional support.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is very little variation in this variable across time.</t>
+  </si>
+  <si>
     <t>violent_crime</t>
   </si>
   <si>
@@ -2313,6 +2400,9 @@
     <t xml:space="preserve">The longitudinal data documentation does not indicate that there should be any breaks in the time trend. This may be because they do not use state sources earlier in the measurement of this variable, but rather they continously use the FBI's Uniform Crime Reports.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are no obvious, discernible disjunctures in the data. Many more states have data available starting in 2012. From 2019 to 2022, there is no variation in the value of this variable.</t>
+  </si>
+  <si>
     <t>access_to_healthy_foods</t>
   </si>
   <si>
@@ -2340,6 +2430,9 @@
     <t xml:space="preserve">The variable is no longer used in the rankings so documentation is more sparse. The data provider recommends the following time comparisons: 2010, 2011-2012. They do not offer reasons as to why.</t>
   </si>
   <si>
+    <t xml:space="preserve">There is a very large, uniform, relative increase in values from 2010 to 2011. Values remain relatively static from 2011 to 2012.</t>
+  </si>
+  <si>
     <t>access_to_recreational_facilities</t>
   </si>
   <si>
@@ -2352,6 +2445,9 @@
     <t xml:space="preserve">The total number of people in a county.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 3 data points available for this variable, and it stopped being updated in 2013.</t>
+  </si>
+  <si>
     <t>fast_food_restaurants</t>
   </si>
   <si>
@@ -2364,6 +2460,9 @@
     <t xml:space="preserve">Total number of restaurants in a county.</t>
   </si>
   <si>
+    <t xml:space="preserve">There are only 2 data points available for this variable, and it stopped being updated in 2013.</t>
+  </si>
+  <si>
     <t>covid-19_age-adjusted_mortality</t>
   </si>
   <si>
@@ -2386,6 +2485,9 @@
   </si>
   <si>
     <t xml:space="preserve">This variable is not used in the rankings so documentation is more sparse. Based on how previous variables from this data source were constructed, it would seem as if the following comparisons should be ok: 2016-2020; 2021-2022, but this is an informed guess.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a very large, uniform, relative increase in values from 2020 to 2021. Unrelated to the data provider recommended break points, there is a large, uniform, relative decline in values from 2022 to 2023.</t>
   </si>
   <si>
     <t>health_care_costs</t>
@@ -3161,8 +3263,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="O1" zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3183,7 +3285,7 @@
     <col customWidth="1" min="15" max="15" style="1" width="26.7109375"/>
     <col customWidth="1" min="16" max="16" style="1" width="63.140625"/>
     <col customWidth="1" min="17" max="17" style="1" width="61.8515625"/>
-    <col customWidth="1" min="18" max="18" style="1" width="58.57421875"/>
+    <col customWidth="1" min="18" max="18" style="1" width="60.421875"/>
     <col min="19" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
@@ -3285,7 +3387,7 @@
       <c r="Q2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="5"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" ht="299.25">
       <c r="A3" s="2" t="s">
@@ -3329,7 +3431,7 @@
         <v>39</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3374,7 +3476,7 @@
       <c r="P4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3420,7 +3522,7 @@
         <v>39</v>
       </c>
       <c r="Q5" s="1"/>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3512,7 +3614,7 @@
       <c r="P7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3560,7 +3662,7 @@
       <c r="Q8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3604,7 +3706,7 @@
         <v>81</v>
       </c>
       <c r="Q9" s="1"/>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3652,7 +3754,7 @@
       <c r="Q10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="R10" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3696,7 +3798,7 @@
       <c r="P11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="R11" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3741,7 +3843,7 @@
       <c r="P12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="R12" s="1" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3785,7 +3887,7 @@
         <v>110</v>
       </c>
       <c r="Q13" s="1"/>
-      <c r="R13" s="5" t="s">
+      <c r="R13" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3993,7 +4095,7 @@
       <c r="P18" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="1" t="s">
         <v>154</v>
       </c>
     </row>
@@ -4042,7 +4144,7 @@
       <c r="P19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="R19" s="1" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4136,7 +4238,7 @@
       <c r="P21" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="R21" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4144,7 +4246,7 @@
       <c r="A22" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>185</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -4168,7 +4270,7 @@
       <c r="J22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K22" s="5" t="s">
         <v>191</v>
       </c>
       <c r="L22" s="1"/>
@@ -4184,7 +4286,7 @@
       <c r="Q22" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="R22" s="5" t="s">
+      <c r="R22" s="1" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4230,7 +4332,7 @@
       <c r="Q23" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="R23" s="5" t="s">
+      <c r="R23" s="1" t="s">
         <v>204</v>
       </c>
     </row>
@@ -4396,13 +4498,13 @@
       <c r="N28" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="O28" s="5" t="s">
+      <c r="O28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="R28" s="5" t="s">
+      <c r="R28" s="1" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4507,7 +4609,7 @@
       <c r="P31" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="R31" s="5" t="s">
+      <c r="R31" s="1" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4545,7 +4647,7 @@
       <c r="P32" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R32" s="5" t="s">
+      <c r="R32" s="1" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4580,7 +4682,7 @@
       <c r="P33" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="R33" s="5" t="s">
+      <c r="R33" s="1" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4615,7 +4717,7 @@
       <c r="O34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R34" s="5" t="s">
+      <c r="R34" s="1" t="s">
         <v>277</v>
       </c>
     </row>
@@ -4694,7 +4796,7 @@
       <c r="P36" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="R36" s="5" t="s">
+      <c r="R36" s="1" t="s">
         <v>291</v>
       </c>
     </row>
@@ -4726,7 +4828,7 @@
       <c r="O37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R37" s="5" t="s">
+      <c r="R37" s="1" t="s">
         <v>294</v>
       </c>
     </row>
@@ -4758,7 +4860,7 @@
       <c r="O38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R38" s="5" t="s">
+      <c r="R38" s="1" t="s">
         <v>294</v>
       </c>
     </row>
@@ -4793,7 +4895,7 @@
       <c r="O39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R39" s="5" t="s">
+      <c r="R39" s="1" t="s">
         <v>304</v>
       </c>
     </row>
@@ -4834,7 +4936,7 @@
       <c r="P40" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="R40" s="5" t="s">
+      <c r="R40" s="1" t="s">
         <v>313</v>
       </c>
     </row>
@@ -4904,7 +5006,7 @@
       <c r="O42" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P42" s="5" t="s">
+      <c r="P42" s="1" t="s">
         <v>326</v>
       </c>
     </row>
@@ -5111,7 +5213,7 @@
       <c r="O48" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R48" s="5" t="s">
+      <c r="R48" s="1" t="s">
         <v>352</v>
       </c>
     </row>
@@ -5190,7 +5292,7 @@
       <c r="O50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R50" s="5" t="s">
+      <c r="R50" s="1" t="s">
         <v>363</v>
       </c>
     </row>
@@ -5231,7 +5333,7 @@
       <c r="P51" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="R51" s="5" t="s">
+      <c r="R51" s="1" t="s">
         <v>368</v>
       </c>
     </row>
@@ -5272,7 +5374,7 @@
       <c r="P52" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="R52" s="5" t="s">
+      <c r="R52" s="1" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5316,11 +5418,11 @@
       <c r="P53" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="R53" s="5" t="s">
+      <c r="R53" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="54" ht="99.75">
+    <row r="54" ht="71.25">
       <c r="A54" s="2" t="s">
         <v>379</v>
       </c>
@@ -5357,10 +5459,10 @@
       <c r="O54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="P54" s="5" t="s">
+      <c r="P54" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="R54" s="5" t="s">
+      <c r="R54" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -5401,7 +5503,7 @@
       <c r="P55" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="R55" s="5" t="s">
+      <c r="R55" s="1" t="s">
         <v>396</v>
       </c>
     </row>
@@ -5439,7 +5541,7 @@
       <c r="O56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R56" s="5" t="s">
+      <c r="R56" s="1" t="s">
         <v>405</v>
       </c>
     </row>
@@ -5519,7 +5621,7 @@
       <c r="P58" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="R58" s="5" t="s">
+      <c r="R58" s="1" t="s">
         <v>416</v>
       </c>
     </row>
@@ -5657,31 +5759,34 @@
         <v>433</v>
       </c>
       <c r="Q62" s="1"/>
+      <c r="R62" s="1" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="63" ht="213.75">
       <c r="A63" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I63" s="1">
         <v>0</v>
@@ -5690,21 +5795,24 @@
         <v>36</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O63" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="64" ht="42.75">
       <c r="A64" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>218</v>
@@ -5713,13 +5821,13 @@
         <v>219</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -5731,24 +5839,27 @@
         <v>38</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="2" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="G65" t="s">
         <v>414</v>
@@ -5763,27 +5874,30 @@
         <v>44</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="O65" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R65" s="1" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="G66" t="s">
         <v>414</v>
@@ -5798,24 +5912,27 @@
         <v>44</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="O66" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R66" s="1" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="2" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>78</v>
@@ -5830,27 +5947,30 @@
         <v>79</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="O67" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R67" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="68" ht="14.25">
       <c r="A68" s="2" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>414</v>
@@ -5868,13 +5988,16 @@
       <c r="O68" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R68" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="69" ht="14.25">
       <c r="A69" s="2" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>218</v>
@@ -5883,10 +6006,10 @@
         <v>219</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
@@ -5895,18 +6018,21 @@
         <v>250</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="O69" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R69" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="70" ht="14.25">
       <c r="A70" s="2" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>238</v>
@@ -5916,7 +6042,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>78</v>
@@ -5931,7 +6057,7 @@
         <v>44</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>58</v>
@@ -5939,19 +6065,19 @@
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="2" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>78</v>
@@ -5966,36 +6092,39 @@
         <v>79</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>484</v>
+        <v>489</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="2" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="I72" s="1">
         <v>0</v>
@@ -6004,36 +6133,39 @@
         <v>36</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="O72" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>491</v>
+        <v>497</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="2" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="G73" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="I73" s="1">
         <v>0</v>
@@ -6042,18 +6174,21 @@
         <v>36</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="O73" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R73" s="1" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="74" ht="14.25">
       <c r="A74" s="2" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>218</v>
@@ -6074,21 +6209,24 @@
         <v>79</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="O74" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R74" s="1" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="75" ht="14.25">
       <c r="A75" s="2" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>218</v>
@@ -6121,28 +6259,31 @@
       <c r="P75" s="1" t="s">
         <v>414</v>
       </c>
+      <c r="R75" s="1" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="76" ht="14.25">
       <c r="A76" s="2" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="I76" s="1">
         <v>0</v>
@@ -6150,34 +6291,40 @@
       <c r="J76" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="K76" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="N76" s="1" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="O76" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>510</v>
+        <v>521</v>
+      </c>
+      <c r="R76" s="5" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="77" ht="14.25">
       <c r="A77" s="2" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="I77" s="1">
         <v>0</v>
@@ -6185,22 +6332,28 @@
       <c r="J77" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="K77" s="1" t="s">
+        <v>529</v>
+      </c>
       <c r="N77" s="1" t="s">
-        <v>517</v>
+        <v>530</v>
       </c>
       <c r="O77" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>518</v>
+        <v>531</v>
+      </c>
+      <c r="R77" s="5" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" s="2" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>520</v>
+        <v>534</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>20</v>
@@ -6212,10 +6365,10 @@
         <v>22</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>521</v>
+        <v>535</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="I78" s="1">
         <v>0</v>
@@ -6224,21 +6377,24 @@
         <v>25</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>523</v>
+        <v>537</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="O78" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R78" s="1" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="79" ht="14.25">
       <c r="A79" s="2" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>526</v>
+        <v>541</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>20</v>
@@ -6250,10 +6406,10 @@
         <v>22</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>528</v>
+        <v>543</v>
       </c>
       <c r="I79" s="1">
         <v>1</v>
@@ -6262,10 +6418,10 @@
         <v>25</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>529</v>
+        <v>544</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>530</v>
+        <v>545</v>
       </c>
       <c r="O79" s="1" t="s">
         <v>58</v>
@@ -6273,7 +6429,7 @@
     </row>
     <row r="80" ht="14.25">
       <c r="A80" s="2" t="s">
-        <v>531</v>
+        <v>546</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>414</v>
@@ -6298,7 +6454,7 @@
         <v>414</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="L80" s="1"/>
       <c r="N80" s="1"/>
@@ -6308,13 +6464,16 @@
       <c r="P80" s="1" t="s">
         <v>414</v>
       </c>
+      <c r="R80" s="1" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="81" ht="14.25">
       <c r="A81" s="2" t="s">
-        <v>533</v>
+        <v>549</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>534</v>
+        <v>550</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>20</v>
@@ -6326,10 +6485,10 @@
         <v>22</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>535</v>
+        <v>551</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>536</v>
+        <v>552</v>
       </c>
       <c r="I81" s="1">
         <v>0</v>
@@ -6338,10 +6497,10 @@
         <v>25</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>537</v>
+        <v>553</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>538</v>
+        <v>554</v>
       </c>
       <c r="O81" s="1" t="s">
         <v>58</v>
@@ -6349,10 +6508,10 @@
     </row>
     <row r="82" ht="14.25">
       <c r="A82" s="2" t="s">
-        <v>539</v>
+        <v>555</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>20</v>
@@ -6364,13 +6523,13 @@
         <v>22</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>541</v>
+        <v>557</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="I82" s="1">
         <v>0</v>
@@ -6379,39 +6538,42 @@
         <v>25</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>545</v>
+        <v>561</v>
       </c>
       <c r="O82" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>546</v>
+        <v>562</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="2" t="s">
-        <v>547</v>
+        <v>564</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>548</v>
+        <v>565</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>549</v>
+        <v>566</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>550</v>
+        <v>567</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>551</v>
+        <v>568</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>552</v>
+        <v>569</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>553</v>
+        <v>570</v>
       </c>
       <c r="I83" s="1">
         <v>0</v>
@@ -6420,36 +6582,39 @@
         <v>25</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>554</v>
+        <v>571</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>555</v>
+        <v>572</v>
       </c>
       <c r="O83" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>556</v>
+        <v>573</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="2" t="s">
-        <v>557</v>
+        <v>574</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>558</v>
+        <v>575</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>549</v>
+        <v>566</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>550</v>
+        <v>567</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>560</v>
+        <v>577</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>78</v>
@@ -6458,42 +6623,45 @@
         <v>0</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>562</v>
+        <v>579</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>555</v>
+        <v>572</v>
       </c>
       <c r="O84" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>556</v>
+        <v>573</v>
+      </c>
+      <c r="R84" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="2" t="s">
-        <v>564</v>
+        <v>581</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>565</v>
+        <v>582</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>549</v>
+        <v>566</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>550</v>
+        <v>567</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>566</v>
+        <v>583</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>78</v>
@@ -6502,42 +6670,45 @@
         <v>0</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>562</v>
+        <v>579</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>555</v>
+        <v>572</v>
       </c>
       <c r="O85" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>556</v>
+        <v>573</v>
+      </c>
+      <c r="R85" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="2" t="s">
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>568</v>
+        <v>585</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>569</v>
+        <v>586</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>570</v>
+        <v>587</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>571</v>
+        <v>588</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>572</v>
+        <v>589</v>
       </c>
       <c r="I86" s="1">
         <v>0</v>
@@ -6546,21 +6717,24 @@
         <v>44</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>573</v>
+        <v>590</v>
       </c>
       <c r="O86" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>574</v>
+        <v>591</v>
+      </c>
+      <c r="R86" s="1" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="2" t="s">
-        <v>575</v>
+        <v>593</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>576</v>
+        <v>594</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>218</v>
@@ -6569,10 +6743,10 @@
         <v>247</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>577</v>
+        <v>595</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>578</v>
+        <v>596</v>
       </c>
       <c r="I87" s="1">
         <v>0</v>
@@ -6586,10 +6760,10 @@
     </row>
     <row r="88" ht="14.25">
       <c r="A88" s="2" t="s">
-        <v>579</v>
+        <v>597</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>580</v>
+        <v>598</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>218</v>
@@ -6598,10 +6772,10 @@
         <v>247</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>581</v>
+        <v>599</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>582</v>
+        <v>600</v>
       </c>
       <c r="I88" s="1">
         <v>0</v>
@@ -6613,15 +6787,18 @@
         <v>69</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>583</v>
+        <v>601</v>
+      </c>
+      <c r="R88" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="2" t="s">
-        <v>584</v>
+        <v>602</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>218</v>
@@ -6630,7 +6807,7 @@
         <v>247</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>586</v>
+        <v>604</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>319</v>
@@ -6644,25 +6821,26 @@
       <c r="O89" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R89" s="1"/>
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="2" t="s">
-        <v>587</v>
+        <v>605</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>588</v>
+        <v>606</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>589</v>
+        <v>607</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>590</v>
+        <v>608</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>591</v>
+        <v>609</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>592</v>
+        <v>610</v>
       </c>
       <c r="I90" s="1">
         <v>0</v>
@@ -6673,25 +6851,28 @@
       <c r="O90" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R90" s="1" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="2" t="s">
-        <v>593</v>
+        <v>612</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>594</v>
+        <v>613</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>595</v>
+        <v>614</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>596</v>
+        <v>615</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>597</v>
+        <v>616</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>598</v>
+        <v>617</v>
       </c>
       <c r="I91" s="1">
         <v>0</v>
@@ -6702,19 +6883,22 @@
       <c r="O91" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R91" s="1" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="1" t="s">
-        <v>599</v>
+        <v>618</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>600</v>
+        <v>619</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>78</v>
@@ -6726,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="O92" s="1" t="s">
         <v>58</v>
@@ -6734,22 +6918,22 @@
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="1" t="s">
-        <v>603</v>
+        <v>622</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>604</v>
+        <v>623</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>605</v>
+        <v>624</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I93" s="1">
         <v>0</v>
@@ -6763,22 +6947,22 @@
     </row>
     <row r="94" ht="14.25">
       <c r="A94" s="1" t="s">
-        <v>607</v>
+        <v>626</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>608</v>
+        <v>627</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>609</v>
+        <v>628</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I94" s="1">
         <v>0</v>
@@ -6792,22 +6976,22 @@
     </row>
     <row r="95" ht="14.25">
       <c r="A95" s="1" t="s">
-        <v>610</v>
+        <v>629</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>611</v>
+        <v>630</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>612</v>
+        <v>631</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I95" s="1">
         <v>0</v>
@@ -6816,7 +7000,7 @@
         <v>36</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>613</v>
+        <v>632</v>
       </c>
       <c r="O95" s="1" t="s">
         <v>58</v>
@@ -6824,22 +7008,22 @@
     </row>
     <row r="96" ht="14.25">
       <c r="A96" s="1" t="s">
-        <v>614</v>
+        <v>633</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>615</v>
+        <v>634</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>616</v>
+        <v>635</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I96" s="1">
         <v>0</v>
@@ -6848,7 +7032,7 @@
         <v>36</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>617</v>
+        <v>636</v>
       </c>
       <c r="O96" s="1" t="s">
         <v>58</v>
@@ -6856,22 +7040,22 @@
     </row>
     <row r="97" ht="14.25">
       <c r="A97" s="1" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>619</v>
+        <v>638</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>620</v>
+        <v>639</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I97" s="1">
         <v>0</v>
@@ -6885,22 +7069,22 @@
     </row>
     <row r="98" ht="14.25">
       <c r="A98" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>602</v>
-      </c>
       <c r="G98" s="1" t="s">
-        <v>623</v>
+        <v>642</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I98" s="1">
         <v>0</v>
@@ -6909,7 +7093,7 @@
         <v>36</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>624</v>
+        <v>643</v>
       </c>
       <c r="O98" s="1" t="s">
         <v>58</v>
@@ -6917,22 +7101,22 @@
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>606</v>
       </c>
       <c r="I99" s="1">
         <v>0</v>
@@ -6946,22 +7130,22 @@
     </row>
     <row r="100" ht="14.25">
       <c r="A100" s="1" t="s">
-        <v>628</v>
+        <v>647</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>629</v>
+        <v>648</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>630</v>
+        <v>649</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I100" s="1">
         <v>0</v>
@@ -6975,10 +7159,10 @@
     </row>
     <row r="101" ht="14.25">
       <c r="A101" s="1" t="s">
-        <v>631</v>
+        <v>650</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>632</v>
+        <v>651</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>218</v>
@@ -6988,10 +7172,10 @@
       </c>
       <c r="E101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>633</v>
+        <v>652</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I101" s="1">
         <v>0</v>
@@ -7004,25 +7188,28 @@
         <v>58</v>
       </c>
       <c r="P101" s="1"/>
+      <c r="R101" s="1" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="1" t="s">
-        <v>634</v>
+        <v>654</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>635</v>
+        <v>655</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>636</v>
+        <v>656</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I102" s="1">
         <v>0</v>
@@ -7031,30 +7218,33 @@
         <v>36</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>637</v>
+        <v>657</v>
       </c>
       <c r="O102" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R102" s="1" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="103" ht="14.25">
       <c r="A103" s="1" t="s">
-        <v>638</v>
+        <v>659</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>639</v>
+        <v>660</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>640</v>
+        <v>661</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I103" s="1">
         <v>0</v>
@@ -7065,10 +7255,13 @@
       <c r="O103" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R103" s="1" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="2" t="s">
-        <v>641</v>
+        <v>663</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>414</v>
@@ -7101,15 +7294,18 @@
         <v>69</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>642</v>
+        <v>664</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="105" ht="14.25">
       <c r="A105" s="2" t="s">
-        <v>643</v>
+        <v>666</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>644</v>
+        <v>667</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>218</v>
@@ -7118,10 +7314,10 @@
         <v>247</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>645</v>
+        <v>668</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>646</v>
+        <v>669</v>
       </c>
       <c r="I105" s="1">
         <v>0</v>
@@ -7133,12 +7329,15 @@
         <v>69</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>647</v>
+        <v>670</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="106" ht="14.25">
       <c r="A106" s="2" t="s">
-        <v>648</v>
+        <v>671</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>414</v>
@@ -7167,19 +7366,22 @@
       <c r="P106" s="1" t="s">
         <v>414</v>
       </c>
+      <c r="R106" s="1" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="2" t="s">
-        <v>649</v>
+        <v>673</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>414</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>650</v>
+        <v>674</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>651</v>
+        <v>675</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>414</v>
@@ -7199,25 +7401,28 @@
       <c r="P107" s="1" t="s">
         <v>414</v>
       </c>
+      <c r="R107" s="1" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="2" t="s">
-        <v>652</v>
+        <v>677</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>653</v>
+        <v>678</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>654</v>
+        <v>679</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>655</v>
+        <v>680</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>656</v>
+        <v>681</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="I108" s="1">
         <v>0</v>
@@ -7226,21 +7431,24 @@
         <v>25</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>657</v>
+        <v>682</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>658</v>
+        <v>683</v>
       </c>
       <c r="O108" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R108" s="1" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="2" t="s">
-        <v>659</v>
+        <v>685</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>660</v>
+        <v>686</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>207</v>
@@ -7250,10 +7458,10 @@
       </c>
       <c r="E109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>661</v>
+        <v>687</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>662</v>
+        <v>688</v>
       </c>
       <c r="I109" s="1">
         <v>0</v>
@@ -7269,13 +7477,16 @@
       </c>
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
+      <c r="R109" s="1" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="2" t="s">
-        <v>663</v>
+        <v>690</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>664</v>
+        <v>691</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>207</v>
@@ -7302,13 +7513,16 @@
         <v>58</v>
       </c>
       <c r="P110" s="1"/>
+      <c r="R110" s="1" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="2" t="s">
-        <v>665</v>
+        <v>693</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>666</v>
+        <v>694</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>218</v>
@@ -7317,10 +7531,10 @@
         <v>219</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>667</v>
+        <v>695</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>668</v>
+        <v>696</v>
       </c>
       <c r="I111" s="1">
         <v>0</v>
@@ -7334,13 +7548,16 @@
         <v>58</v>
       </c>
       <c r="P111" s="1"/>
+      <c r="R111" s="1" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="2" t="s">
-        <v>669</v>
+        <v>697</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>670</v>
+        <v>698</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>31</v>
@@ -7352,7 +7569,7 @@
         <v>33</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>671</v>
+        <v>699</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>35</v>
@@ -7371,28 +7588,31 @@
       <c r="O112" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="R112" s="1" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="2" t="s">
-        <v>672</v>
+        <v>701</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>673</v>
+        <v>702</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>674</v>
+        <v>703</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>675</v>
+        <v>704</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>676</v>
+        <v>705</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>677</v>
+        <v>706</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>678</v>
+        <v>707</v>
       </c>
       <c r="I113" s="1">
         <v>0</v>
@@ -7402,37 +7622,40 @@
       </c>
       <c r="K113" s="1"/>
       <c r="N113" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="O113" s="5" t="s">
-        <v>680</v>
+        <v>708</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>709</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>681</v>
+        <v>710</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>682</v>
+        <v>711</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="2" t="s">
-        <v>683</v>
+        <v>713</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>684</v>
+        <v>714</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>685</v>
+        <v>715</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>686</v>
+        <v>716</v>
       </c>
       <c r="E114" s="1"/>
       <c r="G114" s="1" t="s">
-        <v>687</v>
+        <v>717</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>688</v>
+        <v>718</v>
       </c>
       <c r="I114" s="1">
         <v>0</v>
@@ -7441,25 +7664,28 @@
         <v>36</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>689</v>
+        <v>719</v>
       </c>
       <c r="L114" s="1"/>
       <c r="N114" s="1" t="s">
-        <v>690</v>
+        <v>720</v>
       </c>
       <c r="O114" s="1" t="s">
         <v>38</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>691</v>
+        <v>721</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="2" t="s">
-        <v>692</v>
+        <v>723</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>693</v>
+        <v>724</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>272</v>
@@ -7469,10 +7695,10 @@
       </c>
       <c r="E115" s="1"/>
       <c r="G115" s="1" t="s">
-        <v>694</v>
+        <v>725</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>695</v>
+        <v>726</v>
       </c>
       <c r="I115" s="1">
         <v>0</v>
@@ -7487,13 +7713,16 @@
         <v>58</v>
       </c>
       <c r="P115" s="1"/>
+      <c r="R115" s="1" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="2" t="s">
-        <v>696</v>
+        <v>728</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>697</v>
+        <v>729</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>272</v>
@@ -7503,10 +7732,10 @@
       </c>
       <c r="E116" s="1"/>
       <c r="G116" s="1" t="s">
-        <v>698</v>
+        <v>730</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>699</v>
+        <v>731</v>
       </c>
       <c r="I116" s="1">
         <v>0</v>
@@ -7520,13 +7749,16 @@
         <v>58</v>
       </c>
       <c r="P116" s="1"/>
+      <c r="R116" s="1" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="2" t="s">
-        <v>700</v>
+        <v>733</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>701</v>
+        <v>734</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>20</v>
@@ -7536,10 +7768,10 @@
       </c>
       <c r="E117" s="1"/>
       <c r="G117" s="1" t="s">
-        <v>702</v>
+        <v>735</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>695</v>
+        <v>726</v>
       </c>
       <c r="I117" s="1">
         <v>1</v>
@@ -7554,13 +7786,16 @@
         <v>58</v>
       </c>
       <c r="P117" s="1"/>
+      <c r="R117" s="1" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="2" t="s">
-        <v>703</v>
+        <v>736</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>704</v>
+        <v>737</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>31</v>
@@ -7572,10 +7807,10 @@
         <v>33</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>705</v>
+        <v>738</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>706</v>
+        <v>739</v>
       </c>
       <c r="I118" s="1">
         <v>1</v>
@@ -7593,12 +7828,15 @@
         <v>69</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>707</v>
+        <v>740</v>
+      </c>
+      <c r="R118" s="1" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="2" t="s">
-        <v>708</v>
+        <v>742</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>414</v>
@@ -7607,10 +7845,10 @@
         <v>207</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>709</v>
+        <v>743</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>710</v>
+        <v>744</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>414</v>
@@ -7637,7 +7875,7 @@
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="2" t="s">
-        <v>711</v>
+        <v>745</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>414</v>
@@ -7659,7 +7897,7 @@
         <v>414</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O120" s="1" t="s">
         <v>414</v>
@@ -7670,7 +7908,7 @@
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="2" t="s">
-        <v>713</v>
+        <v>747</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>414</v>
@@ -7691,7 +7929,7 @@
         <v>414</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O121" s="1" t="s">
         <v>414</v>
@@ -7702,7 +7940,7 @@
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="2" t="s">
-        <v>714</v>
+        <v>748</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>414</v>
@@ -7723,7 +7961,7 @@
         <v>414</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O122" s="1" t="s">
         <v>414</v>
@@ -7734,7 +7972,7 @@
     </row>
     <row r="123" ht="14.25">
       <c r="A123" s="2" t="s">
-        <v>715</v>
+        <v>749</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>414</v>
@@ -7755,7 +7993,7 @@
         <v>414</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O123" s="1" t="s">
         <v>414</v>
@@ -7766,7 +8004,7 @@
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="2" t="s">
-        <v>716</v>
+        <v>750</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>414</v>
@@ -7787,7 +8025,7 @@
         <v>414</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O124" s="1" t="s">
         <v>414</v>
@@ -7798,7 +8036,7 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="2" t="s">
-        <v>717</v>
+        <v>751</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>414</v>
@@ -7819,7 +8057,7 @@
         <v>414</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O125" s="1" t="s">
         <v>414</v>
@@ -7830,7 +8068,7 @@
     </row>
     <row r="126" ht="14.25">
       <c r="A126" s="2" t="s">
-        <v>718</v>
+        <v>752</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>414</v>
@@ -7851,7 +8089,7 @@
         <v>414</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O126" s="1" t="s">
         <v>414</v>
@@ -7862,7 +8100,7 @@
     </row>
     <row r="127" ht="14.25">
       <c r="A127" s="2" t="s">
-        <v>719</v>
+        <v>753</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>414</v>
@@ -7883,7 +8121,7 @@
         <v>414</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="O127" s="1" t="s">
         <v>414</v>
@@ -7894,7 +8132,7 @@
     </row>
     <row r="128" ht="14.25">
       <c r="A128" s="2" t="s">
-        <v>720</v>
+        <v>754</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>414</v>
@@ -7915,7 +8153,7 @@
         <v>414</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O128" s="1" t="s">
         <v>414</v>
@@ -7926,7 +8164,7 @@
     </row>
     <row r="129" ht="14.25">
       <c r="A129" s="2" t="s">
-        <v>722</v>
+        <v>756</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>414</v>
@@ -7947,7 +8185,7 @@
         <v>414</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O129" s="1" t="s">
         <v>414</v>
@@ -7958,7 +8196,7 @@
     </row>
     <row r="130" ht="14.25">
       <c r="A130" s="2" t="s">
-        <v>723</v>
+        <v>757</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>414</v>
@@ -7979,7 +8217,7 @@
         <v>414</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O130" s="1" t="s">
         <v>414</v>
@@ -7990,7 +8228,7 @@
     </row>
     <row r="131" ht="14.25">
       <c r="A131" s="2" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>414</v>
@@ -8011,7 +8249,7 @@
         <v>414</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O131" s="1" t="s">
         <v>414</v>
@@ -8022,7 +8260,7 @@
     </row>
     <row r="132" ht="14.25">
       <c r="A132" s="2" t="s">
-        <v>725</v>
+        <v>759</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>414</v>
@@ -8043,7 +8281,7 @@
         <v>414</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O132" s="1" t="s">
         <v>414</v>
@@ -8054,7 +8292,7 @@
     </row>
     <row r="133" ht="14.25">
       <c r="A133" s="2" t="s">
-        <v>726</v>
+        <v>760</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>414</v>
@@ -8075,7 +8313,7 @@
         <v>414</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O133" s="1" t="s">
         <v>414</v>
@@ -8086,7 +8324,7 @@
     </row>
     <row r="134" ht="14.25">
       <c r="A134" s="2" t="s">
-        <v>727</v>
+        <v>761</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>414</v>
@@ -8107,7 +8345,7 @@
         <v>414</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="O134" s="1" t="s">
         <v>414</v>
@@ -8118,7 +8356,7 @@
     </row>
     <row r="135" ht="14.25">
       <c r="A135" s="2" t="s">
-        <v>728</v>
+        <v>762</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>414</v>
@@ -8139,7 +8377,7 @@
         <v>414</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O135" s="1" t="s">
         <v>414</v>
@@ -8150,7 +8388,7 @@
     </row>
     <row r="136" ht="14.25">
       <c r="A136" s="2" t="s">
-        <v>730</v>
+        <v>764</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>414</v>
@@ -8171,7 +8409,7 @@
         <v>414</v>
       </c>
       <c r="N136" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O136" s="1" t="s">
         <v>414</v>
@@ -8182,7 +8420,7 @@
     </row>
     <row r="137" ht="14.25">
       <c r="A137" s="2" t="s">
-        <v>731</v>
+        <v>765</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>414</v>
@@ -8203,7 +8441,7 @@
         <v>414</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O137" s="1" t="s">
         <v>414</v>
@@ -8214,7 +8452,7 @@
     </row>
     <row r="138" ht="14.25">
       <c r="A138" s="2" t="s">
-        <v>732</v>
+        <v>766</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>414</v>
@@ -8235,7 +8473,7 @@
         <v>414</v>
       </c>
       <c r="N138" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O138" s="1" t="s">
         <v>414</v>
@@ -8246,7 +8484,7 @@
     </row>
     <row r="139" ht="14.25">
       <c r="A139" s="2" t="s">
-        <v>733</v>
+        <v>767</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>414</v>
@@ -8267,7 +8505,7 @@
         <v>414</v>
       </c>
       <c r="N139" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O139" s="1" t="s">
         <v>414</v>
@@ -8278,7 +8516,7 @@
     </row>
     <row r="140" ht="14.25">
       <c r="A140" s="2" t="s">
-        <v>734</v>
+        <v>768</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>414</v>
@@ -8300,7 +8538,7 @@
       </c>
       <c r="K140" s="1"/>
       <c r="N140" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O140" s="1" t="s">
         <v>414</v>
@@ -8311,7 +8549,7 @@
     </row>
     <row r="141" ht="14.25">
       <c r="A141" s="2" t="s">
-        <v>735</v>
+        <v>769</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>414</v>
@@ -8332,10 +8570,10 @@
         <v>414</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>736</v>
+        <v>770</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O141" s="1" t="s">
         <v>414</v>
@@ -8346,7 +8584,7 @@
     </row>
     <row r="142" ht="14.25">
       <c r="A142" s="2" t="s">
-        <v>737</v>
+        <v>771</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>414</v>
@@ -8367,7 +8605,7 @@
         <v>414</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O142" s="1" t="s">
         <v>414</v>
@@ -8378,7 +8616,7 @@
     </row>
     <row r="143" ht="14.25">
       <c r="A143" s="2" t="s">
-        <v>738</v>
+        <v>772</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>414</v>
@@ -8399,7 +8637,7 @@
         <v>414</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O143" s="1" t="s">
         <v>414</v>
@@ -8410,7 +8648,7 @@
     </row>
     <row r="144" ht="14.25">
       <c r="A144" s="2" t="s">
-        <v>739</v>
+        <v>773</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>414</v>
@@ -8431,7 +8669,7 @@
         <v>414</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O144" s="1" t="s">
         <v>414</v>
@@ -8442,7 +8680,7 @@
     </row>
     <row r="145" ht="14.25">
       <c r="A145" s="2" t="s">
-        <v>740</v>
+        <v>774</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>414</v>
@@ -8463,7 +8701,7 @@
         <v>414</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O145" s="1" t="s">
         <v>414</v>
@@ -8474,7 +8712,7 @@
     </row>
     <row r="146" ht="14.25">
       <c r="A146" s="2" t="s">
-        <v>741</v>
+        <v>775</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>414</v>
@@ -8495,7 +8733,7 @@
         <v>414</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O146" s="1" t="s">
         <v>414</v>
@@ -8506,7 +8744,7 @@
     </row>
     <row r="147" ht="14.25">
       <c r="A147" s="2" t="s">
-        <v>742</v>
+        <v>776</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>414</v>
@@ -8527,7 +8765,7 @@
         <v>414</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O147" s="1" t="s">
         <v>414</v>
@@ -8538,7 +8776,7 @@
     </row>
     <row r="148" ht="14.25">
       <c r="A148" s="2" t="s">
-        <v>743</v>
+        <v>777</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>414</v>
@@ -8559,7 +8797,7 @@
         <v>414</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O148" s="1" t="s">
         <v>414</v>
@@ -8570,7 +8808,7 @@
     </row>
     <row r="149" ht="14.25">
       <c r="A149" s="2" t="s">
-        <v>744</v>
+        <v>778</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>414</v>
@@ -8591,7 +8829,7 @@
         <v>414</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O149" s="1" t="s">
         <v>414</v>
@@ -8602,7 +8840,7 @@
     </row>
     <row r="150" ht="14.25">
       <c r="A150" s="2" t="s">
-        <v>745</v>
+        <v>779</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>414</v>
@@ -8623,7 +8861,7 @@
         <v>414</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O150" s="1" t="s">
         <v>414</v>
@@ -8634,7 +8872,7 @@
     </row>
     <row r="151" ht="14.25">
       <c r="A151" s="2" t="s">
-        <v>746</v>
+        <v>780</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>414</v>
@@ -8655,7 +8893,7 @@
         <v>414</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O151" s="1" t="s">
         <v>414</v>
@@ -8666,7 +8904,7 @@
     </row>
     <row r="152" ht="14.25">
       <c r="A152" s="2" t="s">
-        <v>747</v>
+        <v>781</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>414</v>
@@ -8687,7 +8925,7 @@
         <v>414</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O152" s="1" t="s">
         <v>414</v>
@@ -8698,7 +8936,7 @@
     </row>
     <row r="153" ht="14.25">
       <c r="A153" s="2" t="s">
-        <v>748</v>
+        <v>782</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>414</v>
@@ -8719,7 +8957,7 @@
         <v>414</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O153" s="1" t="s">
         <v>414</v>
@@ -8730,7 +8968,7 @@
     </row>
     <row r="154" ht="14.25">
       <c r="A154" s="2" t="s">
-        <v>749</v>
+        <v>783</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>414</v>
@@ -8751,7 +8989,7 @@
         <v>414</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O154" s="1" t="s">
         <v>414</v>
@@ -8762,7 +9000,7 @@
     </row>
     <row r="155" ht="14.25">
       <c r="A155" s="2" t="s">
-        <v>750</v>
+        <v>784</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>414</v>
@@ -8783,7 +9021,7 @@
         <v>414</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O155" s="1" t="s">
         <v>414</v>
@@ -8794,7 +9032,7 @@
     </row>
     <row r="156" ht="14.25">
       <c r="A156" s="2" t="s">
-        <v>751</v>
+        <v>785</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>414</v>
@@ -8815,7 +9053,7 @@
         <v>414</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O156" s="1" t="s">
         <v>414</v>
@@ -8826,7 +9064,7 @@
     </row>
     <row r="157" ht="14.25">
       <c r="A157" s="2" t="s">
-        <v>752</v>
+        <v>786</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>414</v>
@@ -8847,7 +9085,7 @@
         <v>414</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O157" s="1" t="s">
         <v>414</v>
@@ -8858,7 +9096,7 @@
     </row>
     <row r="158" ht="14.25">
       <c r="A158" s="2" t="s">
-        <v>753</v>
+        <v>787</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>414</v>
@@ -8879,7 +9117,7 @@
         <v>414</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O158" s="1" t="s">
         <v>414</v>
@@ -8890,7 +9128,7 @@
     </row>
     <row r="159" ht="14.25">
       <c r="A159" s="2" t="s">
-        <v>754</v>
+        <v>788</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>414</v>
@@ -8911,7 +9149,7 @@
         <v>414</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O159" s="1" t="s">
         <v>414</v>
@@ -8922,7 +9160,7 @@
     </row>
     <row r="160" ht="14.25">
       <c r="A160" s="2" t="s">
-        <v>755</v>
+        <v>789</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>414</v>
@@ -8943,7 +9181,7 @@
         <v>414</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O160" s="1" t="s">
         <v>414</v>
@@ -8954,7 +9192,7 @@
     </row>
     <row r="161" ht="14.25">
       <c r="A161" s="2" t="s">
-        <v>756</v>
+        <v>790</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>414</v>
@@ -8975,7 +9213,7 @@
         <v>414</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O161" s="1" t="s">
         <v>414</v>
@@ -8986,7 +9224,7 @@
     </row>
     <row r="162" ht="14.25">
       <c r="A162" s="2" t="s">
-        <v>757</v>
+        <v>791</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>414</v>
@@ -9007,7 +9245,7 @@
         <v>414</v>
       </c>
       <c r="N162" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O162" s="1" t="s">
         <v>414</v>
@@ -9018,7 +9256,7 @@
     </row>
     <row r="163" ht="14.25">
       <c r="A163" s="2" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>414</v>
@@ -9039,7 +9277,7 @@
         <v>414</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O163" s="1" t="s">
         <v>414</v>
@@ -9050,7 +9288,7 @@
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="2" t="s">
-        <v>759</v>
+        <v>793</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>414</v>
@@ -9071,7 +9309,7 @@
         <v>414</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O164" s="1" t="s">
         <v>414</v>
@@ -9082,7 +9320,7 @@
     </row>
     <row r="165" ht="14.25">
       <c r="A165" s="2" t="s">
-        <v>760</v>
+        <v>794</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>414</v>
@@ -9103,7 +9341,7 @@
         <v>414</v>
       </c>
       <c r="N165" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O165" s="1" t="s">
         <v>414</v>
@@ -9114,7 +9352,7 @@
     </row>
     <row r="166" ht="14.25">
       <c r="A166" s="2" t="s">
-        <v>761</v>
+        <v>795</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>414</v>
@@ -9135,7 +9373,7 @@
         <v>414</v>
       </c>
       <c r="N166" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O166" s="1" t="s">
         <v>414</v>
@@ -9146,7 +9384,7 @@
     </row>
     <row r="167" ht="14.25">
       <c r="A167" s="2" t="s">
-        <v>762</v>
+        <v>796</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>414</v>
@@ -9167,7 +9405,7 @@
         <v>414</v>
       </c>
       <c r="N167" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O167" s="1" t="s">
         <v>414</v>
@@ -9178,28 +9416,28 @@
     </row>
     <row r="168" ht="14.25">
       <c r="A168" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="N168" s="1" t="s">
         <v>763</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="G168" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="H168" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="I168" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="J168" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="N168" s="1" t="s">
-        <v>729</v>
       </c>
       <c r="O168" s="1" t="s">
         <v>414</v>
@@ -9210,7 +9448,7 @@
     </row>
     <row r="169" ht="14.25">
       <c r="A169" s="2" t="s">
-        <v>764</v>
+        <v>798</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>414</v>
@@ -9231,7 +9469,7 @@
         <v>414</v>
       </c>
       <c r="N169" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O169" s="1" t="s">
         <v>414</v>
@@ -9242,7 +9480,7 @@
     </row>
     <row r="170" ht="14.25">
       <c r="A170" s="2" t="s">
-        <v>765</v>
+        <v>799</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>414</v>
@@ -9263,7 +9501,7 @@
         <v>414</v>
       </c>
       <c r="N170" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O170" s="1" t="s">
         <v>414</v>
@@ -9274,7 +9512,7 @@
     </row>
     <row r="171" ht="14.25">
       <c r="A171" s="2" t="s">
-        <v>766</v>
+        <v>800</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>414</v>
@@ -9295,7 +9533,7 @@
         <v>414</v>
       </c>
       <c r="N171" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O171" s="1" t="s">
         <v>414</v>
@@ -9306,7 +9544,7 @@
     </row>
     <row r="172" ht="14.25">
       <c r="A172" s="2" t="s">
-        <v>767</v>
+        <v>801</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>414</v>
@@ -9327,7 +9565,7 @@
         <v>414</v>
       </c>
       <c r="N172" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O172" s="1" t="s">
         <v>414</v>
@@ -9338,7 +9576,7 @@
     </row>
     <row r="173" ht="14.25">
       <c r="A173" s="2" t="s">
-        <v>768</v>
+        <v>802</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>414</v>
@@ -9359,7 +9597,7 @@
         <v>414</v>
       </c>
       <c r="N173" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O173" s="1" t="s">
         <v>414</v>
@@ -9370,7 +9608,7 @@
     </row>
     <row r="174" ht="14.25">
       <c r="A174" s="2" t="s">
-        <v>769</v>
+        <v>803</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>414</v>
@@ -9391,7 +9629,7 @@
         <v>414</v>
       </c>
       <c r="N174" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O174" s="1" t="s">
         <v>414</v>
@@ -9402,7 +9640,7 @@
     </row>
     <row r="175" ht="14.25">
       <c r="A175" s="2" t="s">
-        <v>770</v>
+        <v>804</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>414</v>
@@ -9423,7 +9661,7 @@
         <v>414</v>
       </c>
       <c r="N175" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O175" s="1" t="s">
         <v>414</v>
@@ -9434,7 +9672,7 @@
     </row>
     <row r="176" ht="14.25">
       <c r="A176" s="2" t="s">
-        <v>771</v>
+        <v>805</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>414</v>
@@ -9455,7 +9693,7 @@
         <v>414</v>
       </c>
       <c r="N176" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O176" s="1" t="s">
         <v>414</v>
@@ -9466,7 +9704,7 @@
     </row>
     <row r="177" ht="14.25">
       <c r="A177" s="2" t="s">
-        <v>772</v>
+        <v>806</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>414</v>
@@ -9487,7 +9725,7 @@
         <v>414</v>
       </c>
       <c r="N177" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O177" s="1" t="s">
         <v>414</v>
@@ -9498,7 +9736,7 @@
     </row>
     <row r="178" ht="14.25">
       <c r="A178" s="2" t="s">
-        <v>773</v>
+        <v>807</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>414</v>
@@ -9519,7 +9757,7 @@
         <v>414</v>
       </c>
       <c r="N178" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O178" s="1" t="s">
         <v>414</v>
@@ -9530,7 +9768,7 @@
     </row>
     <row r="179" ht="14.25">
       <c r="A179" s="2" t="s">
-        <v>774</v>
+        <v>808</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>414</v>
@@ -9551,7 +9789,7 @@
         <v>414</v>
       </c>
       <c r="N179" s="1" t="s">
-        <v>729</v>
+        <v>763</v>
       </c>
       <c r="O179" s="1" t="s">
         <v>414</v>

</xml_diff>